<commit_message>
Removed Signal Tap - Working
</commit_message>
<xml_diff>
--- a/MultiComp_On_RETRO-EP4CE15/FrontPanel01/docs/IOP_CPU.xlsx
+++ b/MultiComp_On_RETRO-EP4CE15/FrontPanel01/docs/IOP_CPU.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="102">
   <si>
     <t xml:space="preserve">INSTRUCTION</t>
   </si>
@@ -157,6 +157,21 @@
   </si>
   <si>
     <t xml:space="preserve">JUMP TO ADDRESS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12-bit Addresses/12-bit offsets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r0-r7 are general purpose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r8 = 0x00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r9 = 0x01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r15 = 0xFFr</t>
   </si>
   <si>
     <t xml:space="preserve">LABEL</t>
@@ -395,7 +410,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -418,6 +433,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -445,13 +464,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="5.04"/>
@@ -856,6 +875,31 @@
       <c r="Q11" s="3"/>
       <c r="R11" s="5" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -897,237 +941,237 @@
   </sheetPr>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="8.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="10.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="13.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="28.3"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="6" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="10.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="13.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="28.3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="7" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>48</v>
+    <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>52</v>
+      <c r="C3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>54</v>
+      <c r="C4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="D9" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="6" t="s">
+      <c r="D10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="6" t="s">
+      <c r="D11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="C12" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>66</v>
+      <c r="E12" s="7" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>69</v>
+      <c r="C13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>70</v>
+      <c r="C14" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>67</v>
+      <c r="C15" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="D15" s="0"/>
-      <c r="E15" s="6" t="s">
-        <v>71</v>
+      <c r="E15" s="7" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>72</v>
+      <c r="C16" s="7" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1148,169 +1192,169 @@
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.47"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>